<commit_message>
typos in PID facets, new plots in OntologyModels
</commit_message>
<xml_diff>
--- a/Scales/Scales.xlsx
+++ b/Scales/Scales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\git\PsychoOntology\Scales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542B6648-6187-406C-B811-72C181CB5347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E6B1F1-D5C7-49A9-B37C-5F5F09FC7B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{A27227EB-415E-4A49-90A3-E0E096C621E7}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="541">
   <si>
     <t>itemID</t>
   </si>
@@ -398,18 +398,12 @@
     <t>PID5BF16</t>
   </si>
   <si>
-    <t>intimicy avoidance</t>
-  </si>
-  <si>
     <t>Ich halte romantische Gefühle lieber aus meinem Leben heraus.</t>
   </si>
   <si>
     <t>PID5BF17</t>
   </si>
   <si>
-    <t>perceptual dysreg</t>
-  </si>
-  <si>
     <t>Es ist komisch, aber manchmal kommt es mir vor, dass alltägliche Gegenstände eine andere Form haben als sonst.</t>
   </si>
   <si>
@@ -1668,6 +1662,15 @@
   </si>
   <si>
     <t xml:space="preserve">People complain about my need to have everything all arranged. </t>
+  </si>
+  <si>
+    <t>perceptual dysregulation</t>
+  </si>
+  <si>
+    <t>anxiousness</t>
+  </si>
+  <si>
+    <t>intimacy avoidance</t>
   </si>
 </sst>
 </file>
@@ -2090,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E33E46E-83B8-48DE-A3D9-C8D6BACCCF36}">
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:F68"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,13 +2118,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2345,7 +2348,7 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2365,7 +2368,7 @@
         <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2385,7 +2388,7 @@
         <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2405,7 +2408,7 @@
         <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2425,7 +2428,7 @@
         <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2445,7 +2448,7 @@
         <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2465,7 +2468,7 @@
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2485,7 +2488,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2505,7 +2508,7 @@
         <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,7 +2528,7 @@
         <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2545,7 +2548,7 @@
         <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,7 +2568,7 @@
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2585,7 +2588,7 @@
         <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2605,7 +2608,7 @@
         <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2625,7 +2628,7 @@
         <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2645,7 +2648,7 @@
         <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2665,7 +2668,7 @@
         <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,7 +2688,7 @@
         <v>64</v>
       </c>
       <c r="F31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2705,7 +2708,7 @@
         <v>66</v>
       </c>
       <c r="F32" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2725,7 +2728,7 @@
         <v>68</v>
       </c>
       <c r="F33" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2745,7 +2748,7 @@
         <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2765,7 +2768,7 @@
         <v>75</v>
       </c>
       <c r="F35" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2785,7 +2788,7 @@
         <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2805,7 +2808,7 @@
         <v>81</v>
       </c>
       <c r="F37" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2825,7 +2828,7 @@
         <v>84</v>
       </c>
       <c r="F38" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2845,7 +2848,7 @@
         <v>87</v>
       </c>
       <c r="F39" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2865,7 +2868,7 @@
         <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2885,7 +2888,7 @@
         <v>93</v>
       </c>
       <c r="F41" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2905,7 +2908,7 @@
         <v>96</v>
       </c>
       <c r="F42" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,7 +2928,7 @@
         <v>99</v>
       </c>
       <c r="F43" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2945,7 +2948,7 @@
         <v>102</v>
       </c>
       <c r="F44" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2965,7 +2968,7 @@
         <v>105</v>
       </c>
       <c r="F45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,7 +2988,7 @@
         <v>108</v>
       </c>
       <c r="F46" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3005,7 +3008,7 @@
         <v>111</v>
       </c>
       <c r="F47" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3025,7 +3028,7 @@
         <v>114</v>
       </c>
       <c r="F48" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3036,41 +3039,41 @@
         <v>70</v>
       </c>
       <c r="C49" t="s">
+        <v>540</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
         <v>116</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
-        <v>117</v>
-      </c>
       <c r="F49" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>538</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F50" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
         <v>70</v>
@@ -3082,15 +3085,15 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F51" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B52" t="s">
         <v>70</v>
@@ -3102,15 +3105,15 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F52" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
         <v>70</v>
@@ -3122,15 +3125,15 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F53" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B54" t="s">
         <v>70</v>
@@ -3142,15 +3145,15 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F54" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
         <v>70</v>
@@ -3162,15 +3165,15 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F55" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B56" t="s">
         <v>70</v>
@@ -3182,15 +3185,15 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F56" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B57" t="s">
         <v>70</v>
@@ -3202,35 +3205,35 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F57" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B58" t="s">
         <v>70</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>539</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F58" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B59" t="s">
         <v>70</v>
@@ -3242,15 +3245,15 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F59" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
@@ -3262,15 +3265,15 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F60" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B61" t="s">
         <v>70</v>
@@ -3282,55 +3285,55 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F61" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B62" t="s">
         <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F62" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B63" t="s">
         <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F63" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B64" t="s">
         <v>70</v>
@@ -3342,15 +3345,15 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F64" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
@@ -3362,15 +3365,15 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F65" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B66" t="s">
         <v>70</v>
@@ -3382,2648 +3385,2648 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F66" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>540</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F67" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>538</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F68" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B69" t="s">
         <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F69" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>159</v>
+      </c>
+      <c r="B70" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" t="s">
         <v>161</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
         <v>162</v>
-      </c>
-      <c r="C70" t="s">
-        <v>163</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C75" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>173</v>
+      </c>
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" t="s">
+        <v>174</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
         <v>175</v>
-      </c>
-      <c r="B76" t="s">
-        <v>162</v>
-      </c>
-      <c r="C76" t="s">
-        <v>176</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C77" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C78" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C79" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C80" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B82" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C82" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D82">
         <v>-1</v>
       </c>
       <c r="E82" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F82" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>189</v>
+      </c>
+      <c r="B83" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
         <v>191</v>
       </c>
-      <c r="B83" t="s">
-        <v>189</v>
-      </c>
-      <c r="C83" t="s">
-        <v>192</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
-      </c>
-      <c r="E83" t="s">
-        <v>193</v>
-      </c>
       <c r="F83" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B84" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C84" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D84">
         <v>-1</v>
       </c>
       <c r="E84" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F84" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C85" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F85" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C86" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F86" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C87" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F87" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B88" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C88" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F88" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C89" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D89">
         <v>-1</v>
       </c>
       <c r="E89" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F89" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D90">
         <v>-1</v>
       </c>
       <c r="E90" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F90" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C91" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F91" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F92" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C93" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D93">
         <v>-1</v>
       </c>
       <c r="E93" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F93" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B94" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C94" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F94" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C95" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D95">
         <v>-1</v>
       </c>
       <c r="E95" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F95" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B96" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C96" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D96">
         <v>-1</v>
       </c>
       <c r="E96" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F96" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C97" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D97">
         <v>-1</v>
       </c>
       <c r="E97" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F97" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C98" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D98">
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F98" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C99" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D99">
         <v>-1</v>
       </c>
       <c r="E99" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F99" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C100" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D100">
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F100" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B101" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C101" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F101" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B102" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C102" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D102">
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F102" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B103" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C103" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D103">
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F103" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B104" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C104" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D104">
         <v>-1</v>
       </c>
       <c r="E104" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F104" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B105" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C105" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D105">
         <v>-1</v>
       </c>
       <c r="E105" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F105" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B106" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C106" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D106">
         <v>-1</v>
       </c>
       <c r="E106" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F106" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B107" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C107" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D107">
         <v>-1</v>
       </c>
       <c r="E107" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F107" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C108" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D108">
         <v>-1</v>
       </c>
       <c r="E108" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F108" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B109" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C109" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D109">
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F109" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B110" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C110" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D110">
         <v>-1</v>
       </c>
       <c r="E110" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F110" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B111" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C111" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D111">
         <v>-1</v>
       </c>
       <c r="E111" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F111" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B112" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C112" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D112">
         <v>-1</v>
       </c>
       <c r="E112" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F112" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B113" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C113" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D113">
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F113" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B114" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C114" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D114">
         <v>-1</v>
       </c>
       <c r="E114" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F114" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B115" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C115" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D115">
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F115" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B116" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C116" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D116">
         <v>1</v>
       </c>
       <c r="E116" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F116" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B117" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C117" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D117">
         <v>-1</v>
       </c>
       <c r="E117" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F117" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B118" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C118" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D118">
         <v>1</v>
       </c>
       <c r="E118" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F118" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B119" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C119" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D119">
         <v>-1</v>
       </c>
       <c r="E119" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F119" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B120" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C120" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D120">
         <v>-1</v>
       </c>
       <c r="E120" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F120" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B121" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C121" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D121">
         <v>1</v>
       </c>
       <c r="E121" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F121" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B122" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C122" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D122">
         <v>-1</v>
       </c>
       <c r="E122" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F122" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B123" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C123" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D123">
         <v>-1</v>
       </c>
       <c r="E123" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F123" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B124" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C124" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D124">
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F124" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B125" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C125" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D125">
         <v>-1</v>
       </c>
       <c r="E125" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F125" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B126" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C126" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D126">
         <v>-1</v>
       </c>
       <c r="E126" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F126" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C127" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D127">
         <v>-1</v>
       </c>
       <c r="E127" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F127" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B128" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C128" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D128">
         <v>-1</v>
       </c>
       <c r="E128" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F128" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B129" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C129" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D129">
         <v>-1</v>
       </c>
       <c r="E129" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F129" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B130" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C130" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D130">
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F130" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C131" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D131">
         <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F131" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B132" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C132" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D132">
         <v>-1</v>
       </c>
       <c r="E132" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F132" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B133" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C133" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D133">
         <v>1</v>
       </c>
       <c r="E133" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F133" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B134" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C134" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F134" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B135" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C135" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D135">
         <v>-1</v>
       </c>
       <c r="E135" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F135" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B136" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C136" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D136">
         <v>-1</v>
       </c>
       <c r="E136" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F136" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B137" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C137" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D137">
         <v>-1</v>
       </c>
       <c r="E137" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F137" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B138" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C138" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D138">
         <v>-1</v>
       </c>
       <c r="E138" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F138" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B139" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C139" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D139">
         <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F139" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B140" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C140" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D140">
         <v>-1</v>
       </c>
       <c r="E140" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F140" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B141" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C141" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D141">
         <v>1</v>
       </c>
       <c r="E141" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F141" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B142" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C142" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D142">
         <v>-1</v>
       </c>
       <c r="E142" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F142" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B143" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C143" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D143">
         <v>-1</v>
       </c>
       <c r="E143" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F143" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B144" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C144" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D144">
         <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F144" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B145" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C145" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D145">
         <v>1</v>
       </c>
       <c r="E145" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F145" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B146" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C146" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D146">
         <v>-1</v>
       </c>
       <c r="E146" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F146" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B147" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C147" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D147">
         <v>-1</v>
       </c>
       <c r="E147" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F147" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>320</v>
+      </c>
+      <c r="B148" t="s">
+        <v>321</v>
+      </c>
+      <c r="C148" t="s">
         <v>322</v>
       </c>
-      <c r="B148" t="s">
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148" t="s">
         <v>323</v>
-      </c>
-      <c r="C148" t="s">
-        <v>324</v>
-      </c>
-      <c r="D148">
-        <v>1</v>
-      </c>
-      <c r="E148" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>320</v>
+      </c>
+      <c r="B149" t="s">
+        <v>321</v>
+      </c>
+      <c r="C149" t="s">
         <v>322</v>
       </c>
-      <c r="B149" t="s">
-        <v>323</v>
-      </c>
-      <c r="C149" t="s">
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" t="s">
         <v>324</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="E149" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>320</v>
+      </c>
+      <c r="B150" t="s">
+        <v>321</v>
+      </c>
+      <c r="C150" t="s">
         <v>322</v>
-      </c>
-      <c r="B150" t="s">
-        <v>323</v>
-      </c>
-      <c r="C150" t="s">
-        <v>324</v>
       </c>
       <c r="D150">
         <v>-1</v>
       </c>
       <c r="E150" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>320</v>
+      </c>
+      <c r="B151" t="s">
+        <v>321</v>
+      </c>
+      <c r="C151" t="s">
         <v>322</v>
       </c>
-      <c r="B151" t="s">
-        <v>323</v>
-      </c>
-      <c r="C151" t="s">
-        <v>324</v>
-      </c>
       <c r="D151">
         <v>1</v>
       </c>
       <c r="E151" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>320</v>
+      </c>
+      <c r="B152" t="s">
+        <v>321</v>
+      </c>
+      <c r="C152" t="s">
         <v>322</v>
       </c>
-      <c r="B152" t="s">
-        <v>323</v>
-      </c>
-      <c r="C152" t="s">
-        <v>324</v>
-      </c>
       <c r="D152">
         <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B153" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C153" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D153">
         <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B154" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C154" t="s">
+        <v>329</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+      <c r="E154" t="s">
         <v>331</v>
-      </c>
-      <c r="D154">
-        <v>1</v>
-      </c>
-      <c r="E154" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B155" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C155" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B156" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C156" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D156">
         <v>1</v>
       </c>
       <c r="E156" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B157" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C157" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D157">
         <v>2</v>
       </c>
       <c r="E157" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B158" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C158" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D158">
         <v>2</v>
       </c>
       <c r="E158" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B159" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C159" t="s">
+        <v>336</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159" t="s">
         <v>338</v>
-      </c>
-      <c r="D159">
-        <v>1</v>
-      </c>
-      <c r="E159" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B160" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C160" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D160">
         <v>0</v>
       </c>
       <c r="E160" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B161" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C161" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D161">
         <v>1</v>
       </c>
       <c r="E161" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B162" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C162" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D162">
         <v>2</v>
       </c>
       <c r="E162" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B163" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C163" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D163">
         <v>2</v>
       </c>
       <c r="E163" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B164" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C164" t="s">
+        <v>343</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164" t="s">
         <v>345</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-      <c r="E164" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B165" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C165" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D165">
         <v>0</v>
       </c>
       <c r="E165" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B166" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C166" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D166">
         <v>1</v>
       </c>
       <c r="E166" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B167" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C167" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D167">
         <v>2</v>
       </c>
       <c r="E167" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B168" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C168" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D168">
         <v>2</v>
       </c>
       <c r="E168" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B169" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C169" t="s">
+        <v>350</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169" t="s">
         <v>352</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-      <c r="E169" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B170" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C170" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D170">
         <v>0</v>
       </c>
       <c r="E170" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B171" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C171" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D171">
         <v>1</v>
       </c>
       <c r="E171" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B172" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C172" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D172">
         <v>2</v>
       </c>
       <c r="E172" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B173" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C173" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D173">
         <v>2</v>
       </c>
       <c r="E173" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B174" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C174" t="s">
+        <v>357</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174" t="s">
         <v>359</v>
-      </c>
-      <c r="D174">
-        <v>1</v>
-      </c>
-      <c r="E174" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B175" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C175" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D175">
         <v>0</v>
       </c>
       <c r="E175" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B176" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C176" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D176">
         <v>1</v>
       </c>
       <c r="E176" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B177" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C177" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D177">
         <v>2</v>
       </c>
       <c r="E177" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B178" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C178" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D178">
         <v>2</v>
       </c>
       <c r="E178" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B179" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C179" t="s">
+        <v>364</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179" t="s">
         <v>366</v>
-      </c>
-      <c r="D179">
-        <v>1</v>
-      </c>
-      <c r="E179" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B180" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C180" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D180">
         <v>0</v>
       </c>
       <c r="E180" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B181" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C181" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D181">
         <v>1</v>
       </c>
       <c r="E181" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B182" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C182" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D182">
         <v>2</v>
       </c>
       <c r="E182" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B183" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C183" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D183">
         <v>2</v>
       </c>
       <c r="E183" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B184" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C184" t="s">
+        <v>371</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184" t="s">
         <v>373</v>
-      </c>
-      <c r="D184">
-        <v>1</v>
-      </c>
-      <c r="E184" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B185" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C185" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D185">
         <v>0</v>
       </c>
       <c r="E185" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B186" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C186" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D186">
         <v>1</v>
       </c>
       <c r="E186" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B187" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C187" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D187">
         <v>2</v>
       </c>
       <c r="E187" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B188" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C188" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D188">
         <v>2</v>
       </c>
       <c r="E188" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B189" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C189" t="s">
+        <v>378</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+      <c r="E189" t="s">
         <v>380</v>
-      </c>
-      <c r="D189">
-        <v>1</v>
-      </c>
-      <c r="E189" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B190" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C190" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D190">
         <v>0</v>
       </c>
       <c r="E190" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B191" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C191" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D191">
         <v>1</v>
       </c>
       <c r="E191" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B192" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C192" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D192">
         <v>2</v>
       </c>
       <c r="E192" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B193" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C193" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D193">
         <v>2</v>
       </c>
       <c r="E193" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B194" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C194" t="s">
+        <v>385</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194" t="s">
         <v>387</v>
-      </c>
-      <c r="D194">
-        <v>1</v>
-      </c>
-      <c r="E194" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B195" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C195" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D195">
         <v>0</v>
       </c>
       <c r="E195" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B196" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C196" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D196">
         <v>1</v>
       </c>
       <c r="E196" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B197" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C197" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D197">
         <v>2</v>
       </c>
       <c r="E197" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B198" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C198" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D198">
         <v>-1</v>
       </c>
       <c r="E198" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B199" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C199" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D199">
         <v>0</v>
       </c>
       <c r="E199" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B200" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C200" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D200">
         <v>1</v>
       </c>
       <c r="E200" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B201" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C201" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D201">
         <v>2</v>
       </c>
       <c r="E201" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B202" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C202" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D202">
         <v>-1</v>
       </c>
       <c r="E202" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B203" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C203" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D203">
         <v>0</v>
       </c>
       <c r="E203" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B204" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C204" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D204">
         <v>1</v>
       </c>
       <c r="E204" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B205" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C205" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D205">
         <v>2</v>
       </c>
       <c r="E205" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B206" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C206" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D206">
         <v>-1</v>
       </c>
       <c r="E206" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B207" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C207" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D207">
         <v>0</v>
       </c>
       <c r="E207" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B208" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C208" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D208">
         <v>1</v>
       </c>
       <c r="E208" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B209" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C209" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D209">
         <v>2</v>
       </c>
       <c r="E209" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>